<commit_message>
puan hesaplama 2 init
</commit_message>
<xml_diff>
--- a/content/posts/05_2022_yks_puan hesaplama/sayisal_veriler21.xlsx
+++ b/content/posts/05_2022_yks_puan hesaplama/sayisal_veriler21.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevRSA\D3\content\posts\05_2022_yks_puan hesaplama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8CD6D7-E8ED-4967-8F66-2C1C87DB3DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30543F77-19CF-4167-9A1D-7FF1D903DCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>Türkçe</t>
   </si>
@@ -77,17 +90,6 @@
   </si>
   <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>Aday
-Sayısı*</t>
-  </si>
-  <si>
-    <t>Ortalama</t>
-  </si>
-  <si>
-    <t>Standart
-Sapma</t>
   </si>
   <si>
     <t>TYT</t>
@@ -107,6 +109,24 @@
   </si>
   <si>
     <t>YDT</t>
+  </si>
+  <si>
+    <t>T Aday Sayısı</t>
+  </si>
+  <si>
+    <t>T Ortalama</t>
+  </si>
+  <si>
+    <t>T Standart Sapma</t>
+  </si>
+  <si>
+    <t>SS Aday Sayısı</t>
+  </si>
+  <si>
+    <t>SS Ortalama</t>
+  </si>
+  <si>
+    <t>SS Standart Sapma</t>
   </si>
 </sst>
 </file>
@@ -168,29 +188,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,18 +547,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283C1D0F-4E78-4F22-A13C-AEB0F3D4583B}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -545,18 +570,27 @@
         <v>18</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -570,10 +604,19 @@
       <c r="E2" s="2">
         <v>7.7519999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F2" s="8">
+        <v>935058</v>
+      </c>
+      <c r="G2" s="8">
+        <v>18.738</v>
+      </c>
+      <c r="H2" s="8">
+        <v>7.8810000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -587,10 +630,19 @@
       <c r="E3" s="2">
         <v>4.21</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F3" s="8">
+        <v>935058</v>
+      </c>
+      <c r="G3" s="8">
+        <v>8.5739999999999998</v>
+      </c>
+      <c r="H3" s="8">
+        <v>4.1879999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -604,10 +656,19 @@
       <c r="E4" s="2">
         <v>5.5949999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F4" s="8">
+        <v>935058</v>
+      </c>
+      <c r="G4" s="8">
+        <v>5.5460000000000003</v>
+      </c>
+      <c r="H4" s="8">
+        <v>5.867</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -621,10 +682,19 @@
       <c r="E5" s="2">
         <v>4.0970000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F5" s="8">
+        <v>935058</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3.7959999999999998</v>
+      </c>
+      <c r="H5" s="8">
+        <v>4.3630000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -638,10 +708,19 @@
       <c r="E6" s="2">
         <v>5.29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F6" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G6" s="8">
+        <v>5.9320000000000004</v>
+      </c>
+      <c r="H6" s="8">
+        <v>5.1210000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -655,13 +734,22 @@
       <c r="E7" s="2">
         <v>1.9430000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F7" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1.7769999999999999</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1.863</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="7">
         <v>1627083</v>
@@ -672,10 +760,19 @@
       <c r="E8" s="2">
         <v>1.798</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2.1469999999999998</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.7729999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -689,13 +786,22 @@
       <c r="E9" s="2">
         <v>1.661</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F9" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1.0920000000000001</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1.4950000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="7">
         <v>1627083</v>
@@ -706,10 +812,19 @@
       <c r="E10" s="2">
         <v>2.859</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F10" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G10" s="8">
+        <v>2.7069999999999999</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2.7320000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -723,13 +838,22 @@
       <c r="E11" s="2">
         <v>2.4430000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F11" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1.792</v>
+      </c>
+      <c r="H11" s="8">
+        <v>2.2610000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="7">
         <v>1627083</v>
@@ -740,10 +864,19 @@
       <c r="E12" s="2">
         <v>1.6080000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F12" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1.5369999999999999</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1.5880000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>8</v>
@@ -757,10 +890,19 @@
       <c r="E13" s="2">
         <v>6.7709999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F13" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G13" s="8">
+        <v>5.2939999999999996</v>
+      </c>
+      <c r="H13" s="8">
+        <v>6.923</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -774,10 +916,19 @@
       <c r="E14" s="2">
         <v>2.286</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F14" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1.5640000000000001</v>
+      </c>
+      <c r="H14" s="8">
+        <v>2.383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>10</v>
@@ -791,10 +942,19 @@
       <c r="E15" s="2">
         <v>3.1949999999999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F15" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1.9910000000000001</v>
+      </c>
+      <c r="H15" s="8">
+        <v>3.2679999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>11</v>
@@ -808,10 +968,19 @@
       <c r="E16" s="2">
         <v>3.4590000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F16" s="8">
+        <v>741214</v>
+      </c>
+      <c r="G16" s="8">
+        <v>2.5019999999999998</v>
+      </c>
+      <c r="H16" s="8">
+        <v>3.5510000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>12</v>
@@ -825,10 +994,19 @@
       <c r="E17" s="2">
         <v>21.920999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F17" s="8">
+        <v>754</v>
+      </c>
+      <c r="G17" s="8">
+        <v>43.122999999999998</v>
+      </c>
+      <c r="H17" s="8">
+        <v>22.393000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
@@ -842,10 +1020,19 @@
       <c r="E18" s="2">
         <v>22.774000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F18" s="8">
+        <v>1346</v>
+      </c>
+      <c r="G18" s="8">
+        <v>37.130000000000003</v>
+      </c>
+      <c r="H18" s="8">
+        <v>22.693999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>14</v>
@@ -859,10 +1046,19 @@
       <c r="E19" s="2">
         <v>19.263000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F19" s="8">
+        <v>456</v>
+      </c>
+      <c r="G19" s="8">
+        <v>43.988999999999997</v>
+      </c>
+      <c r="H19" s="8">
+        <v>17.358000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>15</v>
@@ -876,10 +1072,19 @@
       <c r="E20" s="2">
         <v>21.366</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F20" s="8">
+        <v>49625</v>
+      </c>
+      <c r="G20" s="8">
+        <v>39.273000000000003</v>
+      </c>
+      <c r="H20" s="8">
+        <v>21.861000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>16</v>
@@ -892,6 +1097,15 @@
       </c>
       <c r="E21" s="2">
         <v>23.588999999999999</v>
+      </c>
+      <c r="F21" s="8">
+        <v>142</v>
+      </c>
+      <c r="G21" s="8">
+        <v>52.006999999999998</v>
+      </c>
+      <c r="H21" s="8">
+        <v>21.228000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>